<commit_message>
Fix. convert string to double for price
</commit_message>
<xml_diff>
--- a/TestFinancialReport/data/stockInfo20210521.xlsx
+++ b/TestFinancialReport/data/stockInfo20210521.xlsx
@@ -155,10 +155,10 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -170,7 +170,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>616451000</v>
+        <v>616451</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -178,7 +178,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>575514000</v>
+        <v>575514</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -186,7 +186,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>8060647000</v>
+        <v>8060647</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -194,7 +194,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>469771000</v>
+        <v>469771</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -202,7 +202,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>548604000</v>
+        <v>548604</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,7 +210,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>3079553000</v>
+        <v>3079553</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>